<commit_message>
Revert "Radio Button Updated" Revert
This reverts commit 9c2c35c97b3be002beb3c93e8a0d401cbe037263.
</commit_message>
<xml_diff>
--- a/src/main/java/TestSuite/MDOT/TestCases/MDOT/TC_SM_FOU_NacuboSourceProfile_AddNewProfile.xlsx
+++ b/src/main/java/TestSuite/MDOT/TestCases/MDOT/TC_SM_FOU_NacuboSourceProfile_AddNewProfile.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\athakur\Documents\MDOT\rstar\rstars\src\main\java\TestSuite\MDOT\TestCases\MDOT\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{481F1F3D-D479-4167-B00B-E25285FBF65C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{023E40F9-282E-4A0D-9662-318EF4C37E20}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" activeTab="1" xr2:uid="{E48E3DD6-0E9A-4FCA-89BE-6D5DDCF154A0}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{E48E3DD6-0E9A-4FCA-89BE-6D5DDCF154A0}"/>
   </bookViews>
   <sheets>
     <sheet name="TestSteps" sheetId="1" r:id="rId1"/>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="50" uniqueCount="46">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="48" uniqueCount="42">
   <si>
     <t>Keyword</t>
   </si>
@@ -161,18 +161,6 @@
   </si>
   <si>
     <t>AddNewProfile_Nacubo</t>
-  </si>
-  <si>
-    <t>clickRadioButtonByName</t>
-  </si>
-  <si>
-    <t>Radio</t>
-  </si>
-  <si>
-    <t>getData=Radio</t>
-  </si>
-  <si>
-    <t>N</t>
   </si>
 </sst>
 </file>
@@ -227,7 +215,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="5">
+  <borders count="4">
     <border>
       <left/>
       <right/>
@@ -274,23 +262,12 @@
       </bottom>
       <diagonal/>
     </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top/>
-      <bottom/>
-      <diagonal/>
-    </border>
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
@@ -302,7 +279,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="3" xfId="0" quotePrefix="1" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -620,8 +596,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E67FE2C5-0520-49C6-94B1-F01BCA1A7D63}">
   <dimension ref="A1:F12"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C9" sqref="C9"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -752,13 +728,13 @@
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A9" s="2" t="s">
-        <v>42</v>
+        <v>13</v>
       </c>
       <c r="B9" s="2" t="s">
         <v>18</v>
       </c>
       <c r="C9" s="4" t="s">
-        <v>44</v>
+        <v>14</v>
       </c>
       <c r="D9" s="2"/>
       <c r="E9" s="2"/>
@@ -805,10 +781,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E840CE84-E5D9-4CFB-918D-9A37B53B878D}">
-  <dimension ref="A1:J2"/>
+  <dimension ref="A1:I2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J2" sqref="J2"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="F10" sqref="F10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -819,7 +795,7 @@
     <col min="8" max="8" width="13.7265625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
         <v>19</v>
       </c>
@@ -847,11 +823,8 @@
       <c r="I1" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="J1" s="9" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.35">
+    </row>
+    <row r="2" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A2" s="6">
         <v>1</v>
       </c>
@@ -865,7 +838,7 @@
         <v>25</v>
       </c>
       <c r="E2" s="6">
-        <v>2023</v>
+        <v>2024</v>
       </c>
       <c r="F2" s="7" t="s">
         <v>26</v>
@@ -875,9 +848,6 @@
         <v>34</v>
       </c>
       <c r="I2" s="6"/>
-      <c r="J2" t="s">
-        <v>45</v>
-      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>